<commit_message>
Added docket with selenium grid implementation
</commit_message>
<xml_diff>
--- a/Input/TestData.xlsx
+++ b/Input/TestData.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\utkarshsingh\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\utkarshsingh\Project Frameworks\hybrid-test-framework\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25750F6-C8FB-4D44-AC65-801242DAA1DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D348379-B788-4F79-95B3-3F1B7A1947C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TestData!$A$1:$R$48</definedName>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>Test Case</t>
   </si>
@@ -39,20 +40,38 @@
     <t>Password</t>
   </si>
   <si>
-    <t>logInTest</t>
+    <t>signInTest</t>
   </si>
   <si>
-    <t>utkarshpsingh@gmail.com</t>
+    <t>signInTest_01</t>
   </si>
   <si>
-    <t>utkarsh@123</t>
+    <t>standard_user</t>
+  </si>
+  <si>
+    <t>secret_sauce</t>
+  </si>
+  <si>
+    <t>locked_out_user</t>
+  </si>
+  <si>
+    <t>problem_user</t>
+  </si>
+  <si>
+    <t>performance_glitch_user</t>
+  </si>
+  <si>
+    <t>addingTwoItemToCart</t>
+  </si>
+  <si>
+    <t>addingOneItemToCart</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,6 +93,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF484C55"/>
+      <name val="Roboto"/>
     </font>
   </fonts>
   <fills count="5">
@@ -144,9 +174,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -154,6 +181,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -444,7 +472,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A3:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -483,35 +511,35 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>4</v>
+      <c r="B2" s="8" t="s">
+        <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
+      <c r="C2" s="8" t="s">
+        <v>6</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="2"/>
@@ -534,9 +562,15 @@
       <c r="V2" s="3"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A3" s="3"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="3"/>
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>6</v>
+      </c>
       <c r="D3" s="3"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -558,9 +592,15 @@
       <c r="V3" s="3"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A4" s="3"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="3"/>
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>6</v>
+      </c>
       <c r="D4" s="3"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -582,9 +622,15 @@
       <c r="V4" s="3"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A5" s="3"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="3"/>
+      <c r="A5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>6</v>
+      </c>
       <c r="D5" s="3"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -607,7 +653,7 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6" s="3"/>
-      <c r="B6" s="7"/>
+      <c r="B6" s="6"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="2"/>
@@ -631,7 +677,7 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
-      <c r="B7" s="7"/>
+      <c r="B7" s="6"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="2"/>
@@ -655,7 +701,7 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
-      <c r="B8" s="7"/>
+      <c r="B8" s="6"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="2"/>
@@ -679,7 +725,7 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
-      <c r="B9" s="7"/>
+      <c r="B9" s="6"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="2"/>
@@ -703,7 +749,7 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
-      <c r="B10" s="7"/>
+      <c r="B10" s="6"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="2"/>
@@ -727,7 +773,7 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
-      <c r="B11" s="7"/>
+      <c r="B11" s="6"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="2"/>
@@ -751,7 +797,7 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
-      <c r="B12" s="7"/>
+      <c r="B12" s="6"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="2"/>
@@ -775,7 +821,7 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
-      <c r="B13" s="7"/>
+      <c r="B13" s="6"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="2"/>
@@ -799,7 +845,7 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
-      <c r="B14" s="7"/>
+      <c r="B14" s="6"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="2"/>
@@ -823,7 +869,7 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
-      <c r="B15" s="7"/>
+      <c r="B15" s="6"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="2"/>
@@ -847,7 +893,7 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
-      <c r="B16" s="7"/>
+      <c r="B16" s="6"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="2"/>
@@ -871,7 +917,7 @@
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
-      <c r="B17" s="7"/>
+      <c r="B17" s="6"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="2"/>
@@ -895,7 +941,7 @@
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
-      <c r="B18" s="7"/>
+      <c r="B18" s="6"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="2"/>
@@ -919,7 +965,7 @@
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
-      <c r="B19" s="7"/>
+      <c r="B19" s="6"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="2"/>
@@ -943,7 +989,7 @@
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
-      <c r="B20" s="7"/>
+      <c r="B20" s="6"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="2"/>
@@ -967,7 +1013,7 @@
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
-      <c r="B21" s="7"/>
+      <c r="B21" s="6"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="2"/>
@@ -991,7 +1037,7 @@
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
-      <c r="B22" s="7"/>
+      <c r="B22" s="6"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="2"/>
@@ -1015,7 +1061,7 @@
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
-      <c r="B23" s="7"/>
+      <c r="B23" s="6"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="2"/>
@@ -1039,7 +1085,7 @@
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
-      <c r="B24" s="7"/>
+      <c r="B24" s="6"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="2"/>
@@ -1063,7 +1109,7 @@
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
-      <c r="B25" s="7"/>
+      <c r="B25" s="6"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="2"/>
@@ -1087,7 +1133,7 @@
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
-      <c r="B26" s="7"/>
+      <c r="B26" s="6"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="2"/>
@@ -1111,7 +1157,7 @@
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A27" s="3"/>
-      <c r="B27" s="7"/>
+      <c r="B27" s="6"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="2"/>
@@ -1135,7 +1181,7 @@
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
-      <c r="B28" s="7"/>
+      <c r="B28" s="6"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="2"/>
@@ -1159,7 +1205,7 @@
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
-      <c r="B29" s="7"/>
+      <c r="B29" s="6"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="2"/>
@@ -1183,7 +1229,7 @@
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
-      <c r="B30" s="7"/>
+      <c r="B30" s="6"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="2"/>
@@ -1207,7 +1253,7 @@
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
-      <c r="B31" s="7"/>
+      <c r="B31" s="6"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="2"/>
@@ -1231,7 +1277,7 @@
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A32" s="3"/>
-      <c r="B32" s="7"/>
+      <c r="B32" s="6"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="2"/>
@@ -1255,7 +1301,7 @@
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A33" s="3"/>
-      <c r="B33" s="7"/>
+      <c r="B33" s="6"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="2"/>
@@ -1279,7 +1325,7 @@
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A34" s="3"/>
-      <c r="B34" s="7"/>
+      <c r="B34" s="6"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="2"/>
@@ -1303,7 +1349,7 @@
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A35" s="3"/>
-      <c r="B35" s="7"/>
+      <c r="B35" s="6"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="2"/>
@@ -1327,7 +1373,7 @@
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A36" s="3"/>
-      <c r="B36" s="7"/>
+      <c r="B36" s="6"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="2"/>
@@ -1351,7 +1397,7 @@
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A37" s="3"/>
-      <c r="B37" s="7"/>
+      <c r="B37" s="6"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="2"/>
@@ -1375,7 +1421,7 @@
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A38" s="4"/>
-      <c r="B38" s="7"/>
+      <c r="B38" s="6"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="2"/>
@@ -1399,7 +1445,7 @@
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A39" s="3"/>
-      <c r="B39" s="7"/>
+      <c r="B39" s="6"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="2"/>
@@ -1423,7 +1469,7 @@
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A40" s="3"/>
-      <c r="B40" s="7"/>
+      <c r="B40" s="6"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="2"/>
@@ -1447,7 +1493,7 @@
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A41" s="3"/>
-      <c r="B41" s="7"/>
+      <c r="B41" s="6"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="2"/>
@@ -1471,7 +1517,7 @@
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A42" s="3"/>
-      <c r="B42" s="7"/>
+      <c r="B42" s="6"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="2"/>
@@ -1495,7 +1541,7 @@
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A43" s="3"/>
-      <c r="B43" s="7"/>
+      <c r="B43" s="6"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="2"/>
@@ -1504,7 +1550,7 @@
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
-      <c r="K43" s="5"/>
+      <c r="K43" s="2"/>
       <c r="L43" s="2"/>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
@@ -1528,7 +1574,7 @@
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
-      <c r="K44" s="5"/>
+      <c r="K44" s="2"/>
       <c r="L44" s="2"/>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
@@ -1552,7 +1598,7 @@
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
-      <c r="K45" s="5"/>
+      <c r="K45" s="2"/>
       <c r="L45" s="2"/>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
@@ -1576,7 +1622,7 @@
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
-      <c r="K46" s="5"/>
+      <c r="K46" s="2"/>
       <c r="L46" s="2"/>
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
@@ -1591,7 +1637,7 @@
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A47" s="3"/>
-      <c r="B47" s="7"/>
+      <c r="B47" s="6"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
       <c r="E47" s="2"/>
@@ -1614,12 +1660,12 @@
       <c r="V47" s="3"/>
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A48" s="6"/>
-      <c r="B48" s="7"/>
+      <c r="A48" s="5"/>
+      <c r="B48" s="6"/>
       <c r="C48" s="3"/>
-      <c r="D48" s="6"/>
+      <c r="D48" s="5"/>
       <c r="E48" s="2"/>
-      <c r="F48" s="6"/>
+      <c r="F48" s="5"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
@@ -1628,60 +1674,91 @@
       <c r="L48" s="2"/>
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
-      <c r="O48" s="6"/>
-      <c r="P48" s="6"/>
-      <c r="Q48" s="6"/>
-      <c r="R48" s="6"/>
-      <c r="S48" s="6"/>
-      <c r="T48" s="6"/>
-      <c r="U48" s="6"/>
-      <c r="V48" s="6"/>
+      <c r="O48" s="5"/>
+      <c r="P48" s="5"/>
+      <c r="Q48" s="5"/>
+      <c r="R48" s="5"/>
+      <c r="S48" s="5"/>
+      <c r="T48" s="5"/>
+      <c r="U48" s="5"/>
+      <c r="V48" s="5"/>
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A49" s="6"/>
-      <c r="B49" s="6"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
+      <c r="A49" s="5"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
       <c r="F49" s="2"/>
-      <c r="O49" s="6"/>
-      <c r="P49" s="6"/>
-      <c r="Q49" s="6"/>
-      <c r="R49" s="6"/>
-      <c r="S49" s="6"/>
-      <c r="T49" s="6"/>
-      <c r="U49" s="6"/>
-      <c r="V49" s="6"/>
+      <c r="O49" s="5"/>
+      <c r="P49" s="5"/>
+      <c r="Q49" s="5"/>
+      <c r="R49" s="5"/>
+      <c r="S49" s="5"/>
+      <c r="T49" s="5"/>
+      <c r="U49" s="5"/>
+      <c r="V49" s="5"/>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A50" s="6"/>
-      <c r="B50" s="6"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
-      <c r="F50" s="6"/>
-      <c r="G50" s="6"/>
-      <c r="H50" s="6"/>
-      <c r="I50" s="6"/>
-      <c r="J50" s="6"/>
-      <c r="K50" s="6"/>
-      <c r="L50" s="6"/>
-      <c r="M50" s="6"/>
-      <c r="N50" s="6"/>
-      <c r="O50" s="6"/>
-      <c r="P50" s="6"/>
-      <c r="Q50" s="6"/>
-      <c r="R50" s="6"/>
-      <c r="S50" s="6"/>
-      <c r="T50" s="6"/>
-      <c r="U50" s="6"/>
-      <c r="V50" s="6"/>
+      <c r="A50" s="5"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
+      <c r="I50" s="5"/>
+      <c r="J50" s="5"/>
+      <c r="K50" s="5"/>
+      <c r="L50" s="5"/>
+      <c r="M50" s="5"/>
+      <c r="N50" s="5"/>
+      <c r="O50" s="5"/>
+      <c r="P50" s="5"/>
+      <c r="Q50" s="5"/>
+      <c r="R50" s="5"/>
+      <c r="S50" s="5"/>
+      <c r="T50" s="5"/>
+      <c r="U50" s="5"/>
+      <c r="V50" s="5"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P34">
     <sortCondition ref="D1"/>
   </sortState>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F17692F2-0453-4632-BCAB-0F64FF347E38}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>